<commit_message>
Atualizado ICC/IDF_PLJ (transf Pessanha).
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/ICC.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/ICC.XLSX
@@ -168,6 +168,9 @@
     <t>MARCELO L. SANTANA DE CAMPOS</t>
   </si>
   <si>
+    <t>JOSE HENRIQUE PESSANHA CHAGAS</t>
+  </si>
+  <si>
     <t>DEBORA SILVA DE SOUZA VACCARI</t>
   </si>
   <si>
@@ -237,9 +240,6 @@
     <t> </t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>475</t>
   </si>
   <si>
@@ -258,6 +258,9 @@
     <t>3750</t>
   </si>
   <si>
+    <t>3827</t>
+  </si>
+  <si>
     <t>3929</t>
   </si>
   <si>
@@ -271,9 +274,6 @@
   </si>
   <si>
     <t>4060</t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t> </t>

</xml_diff>